<commit_message>
commit my changes after excel workout(apache poi)
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Keywords.xlsx
+++ b/src/test/resources/testData/Keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emirzayev\Documents\Main Framework\YFramework\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\YFrameworkFinalC4\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3AAA2E-B14E-4A4C-80D1-F008D7E764AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5319EB0F-B259-4807-89C6-28DD674FD3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,27 +25,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Michelle</t>
-  </si>
-  <si>
-    <t>Lisa</t>
-  </si>
-  <si>
-    <t>Omar</t>
-  </si>
-  <si>
-    <t>Names</t>
-  </si>
-  <si>
-    <t>Mudriy</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ExpenseName</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>relationshipIndex</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>businessPurpose</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>Yoll Academy</t>
+  </si>
+  <si>
+    <t>Business Lunch</t>
+  </si>
+  <si>
+    <t>projectName</t>
+  </si>
+  <si>
+    <t>MealB project</t>
+  </si>
+  <si>
+    <t>Chipotle</t>
+  </si>
+  <si>
+    <t>Pizza</t>
   </si>
 </sst>
 </file>
@@ -364,43 +382,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.6328125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.453125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.90625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.90625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.54296875" collapsed="false"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>199.99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>